<commit_message>
add pair tests(1.3.6 and 1.3.7) for claim functionality
</commit_message>
<xml_diff>
--- a/docs/Check.xlsx
+++ b/docs/Check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F36B48-E396-4CE3-B286-6FA1D6A50D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B34766-F107-45CF-B38D-E169678A6D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
+    <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Авторизация в приложение под валидными учетными данными</t>
   </si>
@@ -605,7 +605,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,6 +884,9 @@
       <c r="C23" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -894,6 +897,9 @@
       </c>
       <c r="C24" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add tests and methods
</commit_message>
<xml_diff>
--- a/docs/Check.xlsx
+++ b/docs/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B34766-F107-45CF-B38D-E169678A6D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DC75BD-1FFB-4CE2-A3DE-0B979897F8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Авторизация в приложение под валидными учетными данными</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Попытка создания новой заявки с пустыми полями</t>
+  </si>
+  <si>
+    <t>Время комментария не совпадает с текущим на устройстве</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +617,7 @@
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -798,13 +801,13 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -818,7 +821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -832,7 +835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -846,7 +849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -860,7 +863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -874,7 +877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -888,7 +891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -902,7 +905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -912,8 +915,14 @@
       <c r="C25" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -924,16 +933,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -944,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -955,7 +964,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -966,7 +975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
edit first test for news functional and small edit for actions with replace text
</commit_message>
<xml_diff>
--- a/docs/Check.xlsx
+++ b/docs/Check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8D1258-6698-4C5E-8624-D00D381D3086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A02025-4EC5-45F5-BCF7-FA40796AA2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
+    <workbookView xWindow="-25560" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>Авторизация в приложение под валидными учетными данными</t>
   </si>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678B4764-C494-4B32-98C7-81DD5DEC7929}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,6 +961,9 @@
       <c r="C29" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">

</xml_diff>

<commit_message>
add test for newsfunctionality 1.4.5 and add a pair methods
</commit_message>
<xml_diff>
--- a/docs/Check.xlsx
+++ b/docs/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A362CF-14CC-48A3-B264-497B31382DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBA60D0-4514-49FA-97A8-D406C5AEE66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>Авторизация в приложение под валидными учетными данными</t>
   </si>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678B4764-C494-4B32-98C7-81DD5DEC7929}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,8 +1003,11 @@
       <c r="C32" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1014,8 +1017,11 @@
       <c r="C33" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
add last test for news functionality
</commit_message>
<xml_diff>
--- a/docs/Check.xlsx
+++ b/docs/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBA60D0-4514-49FA-97A8-D406C5AEE66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AF3E86-41CB-4018-81CA-0FF9165A2034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{8D7032A7-027B-4F0B-867C-6EC1A1B17744}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>Авторизация в приложение под валидными учетными данными</t>
   </si>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678B4764-C494-4B32-98C7-81DD5DEC7929}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1031,9 @@
       <c r="C34" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>